<commit_message>
ajout ssr, had et psy
</commit_message>
<xml_diff>
--- a/formats/excel/Formats R3A 20.xlsx
+++ b/formats/excel/Formats R3A 20.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Github/formats_pmeasyr/formats/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5CA9B-8BFF-5647-AF07-93ED63D583BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540"/>
+    <workbookView xWindow="460" yWindow="460" windowWidth="27340" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>libelle</t>
   </si>
@@ -136,18 +137,6 @@
     <t>NOORDR</t>
   </si>
   <si>
-    <t xml:space="preserve">Mois de la date de réalisation de l'acte </t>
-  </si>
-  <si>
-    <t>MOIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Année de la date de réalisation de l'acte </t>
-  </si>
-  <si>
-    <t>ANNEE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nature de l’acte </t>
   </si>
   <si>
@@ -209,12 +198,30 @@
   </si>
   <si>
     <t>NOSEQSEJ</t>
+  </si>
+  <si>
+    <t>Index de liaison</t>
+  </si>
+  <si>
+    <t>ILIAISON</t>
+  </si>
+  <si>
+    <t>Code postal de résidence</t>
+  </si>
+  <si>
+    <t>CDPOSTAL</t>
+  </si>
+  <si>
+    <t>Date de l'acte</t>
+  </si>
+  <si>
+    <t>DATEACTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,6 +297,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -581,11 +591,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B21" activeCellId="1" sqref="G1:H1048576 B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,19 +625,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -635,19 +645,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
       <c r="C3">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -655,19 +665,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -675,19 +685,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D5">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -695,19 +705,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -715,19 +725,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="D7">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -735,39 +745,39 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D8">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D9">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -775,39 +785,39 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="D10">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="D11">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -815,19 +825,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="D12">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -835,19 +845,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="D13">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -855,19 +865,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D14">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -875,19 +885,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D15">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -895,19 +905,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="D16">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -915,19 +925,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="D17">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -935,19 +945,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D18">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -955,19 +965,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="D19">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -975,19 +985,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="D20">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -995,99 +1005,99 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="D21">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="D22">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="D23">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>51</v>
+      <c r="A24" t="s">
+        <v>45</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="D24">
-        <v>88</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>52</v>
+        <v>128</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>53</v>
+      <c r="A25" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D25">
-        <v>94</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
+        <v>129</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -1095,35 +1105,55 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="D26">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>97</v>
+        <v>136</v>
+      </c>
+      <c r="D27">
+        <v>137</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28">
+        <v>138</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1133,7 +1163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1145,7 +1175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>